<commit_message>
New Tests added for Allocation Matrix.
</commit_message>
<xml_diff>
--- a/Data Files/GoPro_UI_Allocation.xlsx
+++ b/Data Files/GoPro_UI_Allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutoTest_1\git\PINS_ODT_NEW_TEST\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FFF118-23BF-4EF9-9020-8111537CE67D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0398FB-2A91-44CB-90CC-F4376B83BBB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="3860" windowWidth="16920" windowHeight="10580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verifications" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Score</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>2D</t>
+  </si>
+  <si>
+    <t>1E</t>
   </si>
 </sst>
 </file>
@@ -354,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -378,6 +381,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New test added for Allocation Matrix.
</commit_message>
<xml_diff>
--- a/Data Files/GoPro_UI_Allocation.xlsx
+++ b/Data Files/GoPro_UI_Allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutoTest_1\git\PINS_ODT_NEW_TEST\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0398FB-2A91-44CB-90CC-F4376B83BBB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664FDACA-D735-4F5B-A4FB-559DB4BA5047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="3860" windowWidth="16920" windowHeight="10580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Score</t>
   </si>
@@ -357,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -383,7 +383,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -391,9 +391,17 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>